<commit_message>
Added word oval to top
</commit_message>
<xml_diff>
--- a/scat.xlsx
+++ b/scat.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaida/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shaida/repos/scatcat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B29939-A703-B04C-9156-7767F7977ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4E1204-9C0A-F447-9738-D696D4A4F7ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="6380" windowWidth="28040" windowHeight="17180" xr2:uid="{07763D9D-2A29-B743-BE16-41DB2E116FC1}"/>
+    <workbookView xWindow="6340" yWindow="5300" windowWidth="28040" windowHeight="17180" xr2:uid="{07763D9D-2A29-B743-BE16-41DB2E116FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Monuments</t>
   </si>
   <si>
-    <t>Consonant K</t>
-  </si>
-  <si>
     <t>Words that include the letter K</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>Non-human tv and movie characters</t>
   </si>
   <si>
-    <t>Words with a P</t>
-  </si>
-  <si>
     <t>Words that include the letter P</t>
   </si>
   <si>
@@ -258,6 +252,12 @@
   </si>
   <si>
     <t>Words associated with country music</t>
+  </si>
+  <si>
+    <t>Words with a “P”</t>
+  </si>
+  <si>
+    <t>Consonant “K”</t>
   </si>
 </sst>
 </file>
@@ -632,7 +632,7 @@
   <dimension ref="B4:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:F40"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,7 +646,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="str">
         <f>SUBSTITUTE(B4," ","")</f>
@@ -663,30 +663,30 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" t="s">
         <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" ref="D5:D40" si="0">SUBSTITUTE(B5," ","")</f>
-        <v>ConsonantK</v>
+        <v>Consonant“K”</v>
       </c>
       <c r="E5">
         <f t="shared" ref="E5:E40" si="1">LEN(D5)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ref="F5:F40" si="2">"{""word"": """&amp;B5&amp;""", ""description"": """&amp;C5&amp;"""},"</f>
-        <v>{"word": "Consonant K", "description": "Words that include the letter K"},</v>
+        <v>{"word": "Consonant “K”", "description": "Words that include the letter K"},</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
         <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -703,10 +703,10 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
@@ -723,10 +723,10 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
         <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -743,10 +743,10 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -763,10 +763,10 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -783,10 +783,10 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
         <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -803,10 +803,10 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -823,10 +823,10 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" t="s">
         <v>18</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -843,10 +843,10 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
         <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>21</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -863,10 +863,10 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
         <v>22</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -883,10 +883,10 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" t="s">
         <v>24</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -903,10 +903,10 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
         <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
@@ -923,10 +923,10 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
         <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>29</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
@@ -943,10 +943,10 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
         <v>30</v>
-      </c>
-      <c r="C19" t="s">
-        <v>31</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
@@ -963,10 +963,10 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
         <v>32</v>
-      </c>
-      <c r="C20" t="s">
-        <v>33</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
@@ -983,10 +983,10 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
         <v>34</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
@@ -1003,10 +1003,10 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
         <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>37</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
         <v>38</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
@@ -1043,10 +1043,10 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" t="s">
         <v>40</v>
-      </c>
-      <c r="C24" t="s">
-        <v>41</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
@@ -1063,10 +1063,10 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
         <v>42</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
@@ -1083,10 +1083,10 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
         <v>44</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
@@ -1103,10 +1103,10 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
         <v>46</v>
-      </c>
-      <c r="C27" t="s">
-        <v>47</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
@@ -1123,10 +1123,10 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" t="s">
         <v>48</v>
-      </c>
-      <c r="C28" t="s">
-        <v>49</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
@@ -1143,30 +1143,30 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>WordswithaP</v>
+        <v>Wordswitha“P”</v>
       </c>
       <c r="E29">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="2"/>
-        <v>{"word": "Words with a P", "description": "Words that include the letter P"},</v>
+        <v>{"word": "Words with a “P”", "description": "Words that include the letter P"},</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
@@ -1183,10 +1183,10 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
@@ -1203,10 +1203,10 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="0"/>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
@@ -1243,10 +1243,10 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C34" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
@@ -1263,10 +1263,10 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
@@ -1283,10 +1283,10 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
@@ -1303,10 +1303,10 @@
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
@@ -1323,10 +1323,10 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
@@ -1343,10 +1343,10 @@
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="0"/>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>

</xml_diff>